<commit_message>
modif code + sheet
</commit_message>
<xml_diff>
--- a/my_comptability_sheet.xlsx
+++ b/my_comptability_sheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.101\nas-data-storage\Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ED46AA-1CDF-42B5-89D7-068E2AF3142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A27A42B-0784-4110-8506-C05853C9285F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A66AC59C-1511-4EAB-855A-A3B5807FAC7E}"/>
+    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A66AC59C-1511-4EAB-855A-A3B5807FAC7E}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="2" r:id="rId1"/>
+    <sheet name="Template" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>Mois</t>
   </si>
@@ -80,9 +81,6 @@
     <t>Revenus</t>
   </si>
   <si>
-    <t>Dépenses</t>
-  </si>
-  <si>
     <t>Sommes Annuel</t>
   </si>
   <si>
@@ -96,6 +94,18 @@
   </si>
   <si>
     <t>Bilan</t>
+  </si>
+  <si>
+    <t>Epargne</t>
+  </si>
+  <si>
+    <t>Investissement</t>
+  </si>
+  <si>
+    <t>Dépenses Fixe</t>
+  </si>
+  <si>
+    <t>Reste</t>
   </si>
 </sst>
 </file>
@@ -172,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -180,11 +190,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -202,13 +220,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
+      <xdr:colOff>752474</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>752474</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -225,8 +243,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="752475" y="3810000"/>
-          <a:ext cx="2552700" cy="3419475"/>
+          <a:off x="752474" y="3810000"/>
+          <a:ext cx="5514975" cy="3419475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -361,16 +379,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -385,8 +403,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4067175" y="3810000"/>
-          <a:ext cx="1524000" cy="3419475"/>
+          <a:off x="7048501" y="3819525"/>
+          <a:ext cx="1504950" cy="3419475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -494,24 +512,354 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F16727DF-E41B-4AFF-8B44-FD47F52CA64F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="3810000"/>
+          <a:ext cx="5257800" cy="3438525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Les revenus sont composé:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>- Salaire</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> Revenus de location</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Dividendes</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Intérêts</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Redevances</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Les</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> dépenses sont composé:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Taxes et impôts</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Nourriture</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Loyer</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Vêtements</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>-Transport</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Paiment d'auto</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Paiement d'hypothèque</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="ZoneTexte 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C8FD432-282F-42FF-B8FF-3323CE1AF2AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6772275" y="3810000"/>
+          <a:ext cx="1504950" cy="3419475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Actif:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> Biens fonciers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Valeurs</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Obligations</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Effets</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Propriété intellectuelle</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Passif:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Hypothèque</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Prêt au consommateur</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Prêt pour auto</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0DB2FADA-08AA-4542-A4CE-418D0CF64970}" name="Tableau1" displayName="Tableau1" ref="B4:D16" totalsRowShown="0">
-  <autoFilter ref="B4:D16" xr:uid="{0DB2FADA-08AA-4542-A4CE-418D0CF64970}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0DB2FADA-08AA-4542-A4CE-418D0CF64970}" name="Tableau1" displayName="Tableau1" ref="B4:G16" totalsRowShown="0">
+  <autoFilter ref="B4:G16" xr:uid="{0DB2FADA-08AA-4542-A4CE-418D0CF64970}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5C750B78-6C6C-4B9E-976C-5C5DA455C7C5}" name="Mois"/>
     <tableColumn id="2" xr3:uid="{4D99B79A-18A4-4E89-9841-1DD8BB6F2DA8}" name="Revenus"/>
-    <tableColumn id="3" xr3:uid="{A2F1906F-CFC1-4FB6-AE8C-91A30821E4DA}" name="Dépenses"/>
+    <tableColumn id="4" xr3:uid="{CA083B85-708C-4ABC-AC4F-2C92802F1690}" name="Epargne"/>
+    <tableColumn id="5" xr3:uid="{20414323-E779-41F9-94CD-6FE8D2A11F74}" name="Investissement"/>
+    <tableColumn id="3" xr3:uid="{A2F1906F-CFC1-4FB6-AE8C-91A30821E4DA}" name="Dépenses Fixe"/>
+    <tableColumn id="6" xr3:uid="{79F643A4-E1EE-4C8C-9BEB-34AC20CD2F17}" name="Reste" dataDxfId="1">
+      <calculatedColumnFormula xml:space="preserve"> C5 - D5 -E5 - F5</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A6282EA1-A304-4F53-BBA6-2ECBA80774CD}" name="Tableau3" displayName="Tableau3" ref="F4:G16" totalsRowShown="0">
-  <autoFilter ref="F4:G16" xr:uid="{A6282EA1-A304-4F53-BBA6-2ECBA80774CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A6282EA1-A304-4F53-BBA6-2ECBA80774CD}" name="Tableau3" displayName="Tableau3" ref="I4:J16" totalsRowShown="0">
+  <autoFilter ref="I4:J16" xr:uid="{A6282EA1-A304-4F53-BBA6-2ECBA80774CD}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B9360C4A-76B3-4B95-9E4A-A227D4A0157D}" name="Actif"/>
     <tableColumn id="2" xr3:uid="{115D56F2-B5B8-47F5-9A30-9DDFAA16F7EB}" name="Passif"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3BBF9AC-B6C4-4DB8-89E5-C0BCA3920F90}" name="Tableau13" displayName="Tableau13" ref="B4:G16" totalsRowShown="0">
+  <autoFilter ref="B4:G16" xr:uid="{A3BBF9AC-B6C4-4DB8-89E5-C0BCA3920F90}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B0D100A9-520D-4302-B297-6F12759D160A}" name="Mois"/>
+    <tableColumn id="2" xr3:uid="{D8C441E8-DF2D-4203-9B6A-16932D97D911}" name="Revenus"/>
+    <tableColumn id="4" xr3:uid="{662CDCEE-A5B9-4161-9418-4F5CEC04E56B}" name="Epargne"/>
+    <tableColumn id="5" xr3:uid="{B8F985DC-55CF-4F04-83FA-912E74626E54}" name="Investissement"/>
+    <tableColumn id="3" xr3:uid="{9D052CE7-4D0E-4D6D-BC0D-53F1ECA1C75E}" name="Dépenses Fixe"/>
+    <tableColumn id="6" xr3:uid="{5DC1A6FC-42B5-4802-9EF2-0DEB97687F6E}" name="Reste" dataDxfId="0">
+      <calculatedColumnFormula xml:space="preserve"> C5 - D5 -E5 - F5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BF7DD2DA-D7B3-423E-8041-433C28E9F9C1}" name="Tableau35" displayName="Tableau35" ref="I4:J16" totalsRowShown="0">
+  <autoFilter ref="I4:J16" xr:uid="{BF7DD2DA-D7B3-423E-8041-433C28E9F9C1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{EDFE0E09-B4C2-445E-89A4-44DBD569CBA9}" name="Actif"/>
+    <tableColumn id="2" xr3:uid="{DE3924EB-C094-4B27-B848-4DBC60B03224}" name="Passif"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -814,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786BB131-61FE-40EA-9F47-E9561FBE84F6}">
-  <dimension ref="B2:G18"/>
+  <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,20 +1173,26 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="5"/>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -846,78 +1200,135 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
       </c>
       <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" ref="G5:G16" si="0" xml:space="preserve"> C5 - D5 -E5 - F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="3">
         <f>SUM(C5:C16)</f>
@@ -927,7 +1338,11 @@
         <f>SUM(D5:D16)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="3">
+      <c r="E18" s="3">
+        <f>SUM(E5:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
         <f>SUM(F5:F16)</f>
         <v>0</v>
       </c>
@@ -935,11 +1350,230 @@
         <f>SUM(G5:G16)</f>
         <v>0</v>
       </c>
+      <c r="I18" s="3">
+        <f>SUM(I5:I16)</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f>SUM(J5:J16)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC507B5-DE8D-40E7-BADC-E4DC568785E0}">
+  <dimension ref="B2:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G16" si="0" xml:space="preserve"> C5 - D5 -E5 - F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3">
+        <f>SUM(C5:C16)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f>SUM(D5:D16)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <f>SUM(E5:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f>SUM(F5:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f>SUM(G5:G16)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <f>SUM(I5:I16)</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f>SUM(J5:J16)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>